<commit_message>
#3 - added table loading
</commit_message>
<xml_diff>
--- a/WorkWithTables/test.xlsx
+++ b/WorkWithTables/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="19">
   <si>
     <t>03.02</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Василь</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>Петро</t>
   </si>
   <si>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>Єгор</t>
+  </si>
+  <si>
+    <t>TESTER</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O6"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="15" width="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -499,26 +583,28 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -528,9 +614,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -588,16 +674,21 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -607,9 +698,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -667,16 +758,21 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -686,9 +782,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -746,95 +842,21 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="15" width="7" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>